<commit_message>
reverted back to parallelization by chunks
</commit_message>
<xml_diff>
--- a/data/referee-performance.xlsx
+++ b/data/referee-performance.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="28620" windowHeight="12915"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="28620" windowHeight="12915" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="fasta-method-1" sheetId="1" r:id="rId1"/>
+    <sheet name="fasta-method-2" sheetId="2" r:id="rId2"/>
+    <sheet name="fasta-method-3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="6">
   <si>
     <t>Num procs</t>
   </si>
@@ -34,18 +34,6 @@
   </si>
   <si>
     <t>Virtual memory usage</t>
-  </si>
-  <si>
-    <t>Index reference fasta</t>
-  </si>
-  <si>
-    <t>Calculate scores</t>
-  </si>
-  <si>
-    <t>Fill unmapped positions</t>
-  </si>
-  <si>
-    <t>End program</t>
   </si>
 </sst>
 </file>
@@ -384,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,164 +408,47 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>3</v>
-      </c>
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>3</v>
-      </c>
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>3</v>
-      </c>
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>4</v>
-      </c>
-      <c r="B15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>4</v>
-      </c>
-      <c r="B16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>4</v>
-      </c>
-      <c r="B17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="F1" t="s">
         <v>5</v>
-      </c>
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>5</v>
-      </c>
-      <c r="B19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>5</v>
-      </c>
-      <c r="B20" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>5</v>
-      </c>
-      <c r="B21" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -585,26 +456,45 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>